<commit_message>
minor changes for ui (drop down)
</commit_message>
<xml_diff>
--- a/General Test.xlsx
+++ b/General Test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kellym\Downloads\WebApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-690" yWindow="1170" windowWidth="20115" windowHeight="7815" tabRatio="383" firstSheet="1" activeTab="1"/>
   </bookViews>
@@ -13,7 +18,7 @@
     <sheet name="COMMUNICATION" sheetId="5" r:id="rId4"/>
     <sheet name="LOGIC" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -5785,7 +5790,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
@@ -6457,12 +6462,21 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -6472,27 +6486,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -6523,6 +6516,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6551,6 +6556,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -7033,7 +7041,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7068,7 +7076,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7325,7 +7333,7 @@
       <c r="E2" s="85"/>
       <c r="F2" s="86">
         <f ca="1">TODAY()</f>
-        <v>42129</v>
+        <v>42915</v>
       </c>
       <c r="G2" s="85"/>
       <c r="H2" s="77"/>
@@ -11074,20 +11082,20 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="111" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
@@ -11849,158 +11857,158 @@
       <c r="E66" s="4"/>
     </row>
     <row r="67" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="127" t="s">
+      <c r="B67" s="123" t="s">
         <v>460</v>
       </c>
-      <c r="C67" s="127"/>
-      <c r="D67" s="127"/>
-      <c r="E67" s="127"/>
-      <c r="F67" s="127"/>
-      <c r="G67" s="127"/>
-      <c r="H67" s="127"/>
-      <c r="I67" s="127"/>
-      <c r="J67" s="127"/>
-      <c r="K67" s="127"/>
+      <c r="C67" s="123"/>
+      <c r="D67" s="123"/>
+      <c r="E67" s="123"/>
+      <c r="F67" s="123"/>
+      <c r="G67" s="123"/>
+      <c r="H67" s="123"/>
+      <c r="I67" s="123"/>
+      <c r="J67" s="123"/>
+      <c r="K67" s="123"/>
     </row>
     <row r="68" spans="1:12" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="120" t="s">
+      <c r="B68" s="111" t="s">
         <v>461</v>
       </c>
-      <c r="C68" s="120"/>
-      <c r="D68" s="120"/>
-      <c r="E68" s="120"/>
-      <c r="F68" s="120"/>
-      <c r="G68" s="120"/>
-      <c r="H68" s="120"/>
-      <c r="I68" s="120"/>
-      <c r="J68" s="120"/>
-      <c r="K68" s="120"/>
+      <c r="C68" s="111"/>
+      <c r="D68" s="111"/>
+      <c r="E68" s="111"/>
+      <c r="F68" s="111"/>
+      <c r="G68" s="111"/>
+      <c r="H68" s="111"/>
+      <c r="I68" s="111"/>
+      <c r="J68" s="111"/>
+      <c r="K68" s="111"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C69" s="110">
+      <c r="C69" s="112">
         <v>1</v>
       </c>
-      <c r="D69" s="115" t="s">
+      <c r="D69" s="132" t="s">
         <v>463</v>
       </c>
-      <c r="E69" s="116"/>
-      <c r="F69" s="116"/>
-      <c r="G69" s="116"/>
-      <c r="H69" s="116"/>
-      <c r="I69" s="116"/>
-      <c r="J69" s="116"/>
-      <c r="K69" s="117"/>
+      <c r="E69" s="133"/>
+      <c r="F69" s="133"/>
+      <c r="G69" s="133"/>
+      <c r="H69" s="133"/>
+      <c r="I69" s="133"/>
+      <c r="J69" s="133"/>
+      <c r="K69" s="134"/>
     </row>
     <row r="70" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C70" s="111"/>
-      <c r="D70" s="112" t="s">
+      <c r="C70" s="113"/>
+      <c r="D70" s="117" t="s">
         <v>464</v>
       </c>
-      <c r="E70" s="113"/>
-      <c r="F70" s="113"/>
-      <c r="G70" s="113"/>
-      <c r="H70" s="113"/>
-      <c r="I70" s="113"/>
-      <c r="J70" s="113"/>
-      <c r="K70" s="114"/>
+      <c r="E70" s="118"/>
+      <c r="F70" s="118"/>
+      <c r="G70" s="118"/>
+      <c r="H70" s="118"/>
+      <c r="I70" s="118"/>
+      <c r="J70" s="118"/>
+      <c r="K70" s="119"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C71" s="110">
+      <c r="C71" s="112">
         <v>2</v>
       </c>
-      <c r="D71" s="124" t="s">
+      <c r="D71" s="120" t="s">
         <v>465</v>
       </c>
-      <c r="E71" s="125"/>
-      <c r="F71" s="125"/>
-      <c r="G71" s="125"/>
-      <c r="H71" s="125"/>
-      <c r="I71" s="125"/>
-      <c r="J71" s="125"/>
-      <c r="K71" s="126"/>
+      <c r="E71" s="121"/>
+      <c r="F71" s="121"/>
+      <c r="G71" s="121"/>
+      <c r="H71" s="121"/>
+      <c r="I71" s="121"/>
+      <c r="J71" s="121"/>
+      <c r="K71" s="122"/>
     </row>
     <row r="72" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="111"/>
-      <c r="D72" s="112" t="s">
+      <c r="C72" s="113"/>
+      <c r="D72" s="117" t="s">
         <v>464</v>
       </c>
-      <c r="E72" s="113"/>
-      <c r="F72" s="113"/>
-      <c r="G72" s="113"/>
-      <c r="H72" s="113"/>
-      <c r="I72" s="113"/>
-      <c r="J72" s="113"/>
-      <c r="K72" s="114"/>
+      <c r="E72" s="118"/>
+      <c r="F72" s="118"/>
+      <c r="G72" s="118"/>
+      <c r="H72" s="118"/>
+      <c r="I72" s="118"/>
+      <c r="J72" s="118"/>
+      <c r="K72" s="119"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="110">
+      <c r="C73" s="112">
         <v>3</v>
       </c>
-      <c r="D73" s="133" t="s">
+      <c r="D73" s="129" t="s">
         <v>466</v>
       </c>
-      <c r="E73" s="134"/>
-      <c r="F73" s="134"/>
-      <c r="G73" s="134"/>
-      <c r="H73" s="134"/>
-      <c r="I73" s="134"/>
-      <c r="J73" s="134"/>
-      <c r="K73" s="135"/>
+      <c r="E73" s="130"/>
+      <c r="F73" s="130"/>
+      <c r="G73" s="130"/>
+      <c r="H73" s="130"/>
+      <c r="I73" s="130"/>
+      <c r="J73" s="130"/>
+      <c r="K73" s="131"/>
     </row>
     <row r="74" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C74" s="111"/>
-      <c r="D74" s="128" t="s">
+      <c r="C74" s="113"/>
+      <c r="D74" s="124" t="s">
         <v>467</v>
       </c>
-      <c r="E74" s="129"/>
-      <c r="F74" s="129"/>
-      <c r="G74" s="129"/>
-      <c r="H74" s="129"/>
-      <c r="I74" s="129"/>
-      <c r="J74" s="129"/>
+      <c r="E74" s="125"/>
+      <c r="F74" s="125"/>
+      <c r="G74" s="125"/>
+      <c r="H74" s="125"/>
+      <c r="I74" s="125"/>
+      <c r="J74" s="125"/>
       <c r="K74" s="15"/>
     </row>
     <row r="75" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="26">
         <v>4</v>
       </c>
-      <c r="D75" s="121" t="s">
+      <c r="D75" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="E75" s="122"/>
-      <c r="F75" s="122"/>
-      <c r="G75" s="122"/>
-      <c r="H75" s="122"/>
-      <c r="I75" s="122"/>
-      <c r="J75" s="122"/>
-      <c r="K75" s="123"/>
+      <c r="E75" s="115"/>
+      <c r="F75" s="115"/>
+      <c r="G75" s="115"/>
+      <c r="H75" s="115"/>
+      <c r="I75" s="115"/>
+      <c r="J75" s="115"/>
+      <c r="K75" s="116"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C76" s="110">
+      <c r="C76" s="112">
         <v>5</v>
       </c>
-      <c r="D76" s="130" t="s">
+      <c r="D76" s="126" t="s">
         <v>468</v>
       </c>
-      <c r="E76" s="131"/>
-      <c r="F76" s="131"/>
-      <c r="G76" s="131"/>
-      <c r="H76" s="131"/>
-      <c r="I76" s="131"/>
-      <c r="J76" s="131"/>
-      <c r="K76" s="132"/>
+      <c r="E76" s="127"/>
+      <c r="F76" s="127"/>
+      <c r="G76" s="127"/>
+      <c r="H76" s="127"/>
+      <c r="I76" s="127"/>
+      <c r="J76" s="127"/>
+      <c r="K76" s="128"/>
     </row>
     <row r="77" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="111"/>
-      <c r="D77" s="128" t="s">
+      <c r="C77" s="113"/>
+      <c r="D77" s="124" t="s">
         <v>469</v>
       </c>
-      <c r="E77" s="129"/>
-      <c r="F77" s="129"/>
-      <c r="G77" s="129"/>
-      <c r="H77" s="129"/>
-      <c r="I77" s="129"/>
-      <c r="J77" s="129"/>
+      <c r="E77" s="125"/>
+      <c r="F77" s="125"/>
+      <c r="G77" s="125"/>
+      <c r="H77" s="125"/>
+      <c r="I77" s="125"/>
+      <c r="J77" s="125"/>
       <c r="K77" s="15"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -12027,30 +12035,30 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D83" s="118" t="s">
+      <c r="D83" s="135" t="s">
         <v>473</v>
       </c>
-      <c r="E83" s="118"/>
-      <c r="F83" s="118"/>
-      <c r="G83" s="118"/>
-      <c r="H83" s="118"/>
-      <c r="I83" s="118"/>
-      <c r="J83" s="118"/>
-      <c r="K83" s="118"/>
-      <c r="L83" s="118"/>
+      <c r="E83" s="135"/>
+      <c r="F83" s="135"/>
+      <c r="G83" s="135"/>
+      <c r="H83" s="135"/>
+      <c r="I83" s="135"/>
+      <c r="J83" s="135"/>
+      <c r="K83" s="135"/>
+      <c r="L83" s="135"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D84" s="119" t="s">
+      <c r="D84" s="110" t="s">
         <v>474</v>
       </c>
-      <c r="E84" s="119"/>
-      <c r="F84" s="119"/>
-      <c r="G84" s="119"/>
-      <c r="H84" s="119"/>
-      <c r="I84" s="119"/>
-      <c r="J84" s="119"/>
-      <c r="K84" s="119"/>
-      <c r="L84" s="119"/>
+      <c r="E84" s="110"/>
+      <c r="F84" s="110"/>
+      <c r="G84" s="110"/>
+      <c r="H84" s="110"/>
+      <c r="I84" s="110"/>
+      <c r="J84" s="110"/>
+      <c r="K84" s="110"/>
+      <c r="L84" s="110"/>
     </row>
     <row r="86" spans="1:12" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="3"/>
@@ -12337,6 +12345,8 @@
   </sheetData>
   <sheetProtection password="D855" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="18">
+    <mergeCell ref="D69:K69"/>
+    <mergeCell ref="D83:L83"/>
     <mergeCell ref="D84:L84"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="C73:C74"/>
@@ -12353,8 +12363,6 @@
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="D70:K70"/>
-    <mergeCell ref="D69:K69"/>
-    <mergeCell ref="D83:L83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" orientation="portrait" r:id="rId1"/>
@@ -14985,21 +14993,21 @@
       </c>
     </row>
     <row r="3" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="123" t="s">
         <v>760</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
     </row>
     <row r="4" spans="2:14" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="37"/>
@@ -15016,21 +15024,21 @@
       <c r="M4" s="37"/>
     </row>
     <row r="5" spans="2:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="111" t="s">
         <v>761</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="120"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="111"/>
     </row>
     <row r="6" spans="2:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
@@ -15191,21 +15199,21 @@
       </c>
     </row>
     <row r="76" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="127" t="s">
+      <c r="B76" s="123" t="s">
         <v>764</v>
       </c>
-      <c r="C76" s="127"/>
-      <c r="D76" s="127"/>
-      <c r="E76" s="127"/>
-      <c r="F76" s="127"/>
-      <c r="G76" s="127"/>
-      <c r="H76" s="127"/>
-      <c r="I76" s="127"/>
-      <c r="J76" s="127"/>
-      <c r="K76" s="127"/>
-      <c r="L76" s="127"/>
-      <c r="M76" s="127"/>
-      <c r="N76" s="127"/>
+      <c r="C76" s="123"/>
+      <c r="D76" s="123"/>
+      <c r="E76" s="123"/>
+      <c r="F76" s="123"/>
+      <c r="G76" s="123"/>
+      <c r="H76" s="123"/>
+      <c r="I76" s="123"/>
+      <c r="J76" s="123"/>
+      <c r="K76" s="123"/>
+      <c r="L76" s="123"/>
+      <c r="M76" s="123"/>
+      <c r="N76" s="123"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B77" s="37"/>
@@ -15222,21 +15230,21 @@
       <c r="M77" s="37"/>
     </row>
     <row r="78" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="120" t="s">
+      <c r="B78" s="111" t="s">
         <v>765</v>
       </c>
-      <c r="C78" s="120"/>
-      <c r="D78" s="120"/>
-      <c r="E78" s="120"/>
-      <c r="F78" s="120"/>
-      <c r="G78" s="120"/>
-      <c r="H78" s="120"/>
-      <c r="I78" s="120"/>
-      <c r="J78" s="120"/>
-      <c r="K78" s="120"/>
-      <c r="L78" s="120"/>
-      <c r="M78" s="120"/>
-      <c r="N78" s="120"/>
+      <c r="C78" s="111"/>
+      <c r="D78" s="111"/>
+      <c r="E78" s="111"/>
+      <c r="F78" s="111"/>
+      <c r="G78" s="111"/>
+      <c r="H78" s="111"/>
+      <c r="I78" s="111"/>
+      <c r="J78" s="111"/>
+      <c r="K78" s="111"/>
+      <c r="L78" s="111"/>
+      <c r="M78" s="111"/>
+      <c r="N78" s="111"/>
     </row>
     <row r="79" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="9" t="s">
@@ -15291,21 +15299,21 @@
       </c>
     </row>
     <row r="117" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="120" t="s">
+      <c r="B117" s="111" t="s">
         <v>767</v>
       </c>
-      <c r="C117" s="120"/>
-      <c r="D117" s="120"/>
-      <c r="E117" s="120"/>
-      <c r="F117" s="120"/>
-      <c r="G117" s="120"/>
-      <c r="H117" s="120"/>
-      <c r="I117" s="120"/>
-      <c r="J117" s="120"/>
-      <c r="K117" s="120"/>
-      <c r="L117" s="120"/>
-      <c r="M117" s="120"/>
-      <c r="N117" s="120"/>
+      <c r="C117" s="111"/>
+      <c r="D117" s="111"/>
+      <c r="E117" s="111"/>
+      <c r="F117" s="111"/>
+      <c r="G117" s="111"/>
+      <c r="H117" s="111"/>
+      <c r="I117" s="111"/>
+      <c r="J117" s="111"/>
+      <c r="K117" s="111"/>
+      <c r="L117" s="111"/>
+      <c r="M117" s="111"/>
+      <c r="N117" s="111"/>
     </row>
     <row r="118" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="9" t="s">
@@ -15372,21 +15380,21 @@
       </c>
     </row>
     <row r="162" spans="2:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="127" t="s">
+      <c r="B162" s="123" t="s">
         <v>769</v>
       </c>
-      <c r="C162" s="127"/>
-      <c r="D162" s="127"/>
-      <c r="E162" s="127"/>
-      <c r="F162" s="127"/>
-      <c r="G162" s="127"/>
-      <c r="H162" s="127"/>
-      <c r="I162" s="127"/>
-      <c r="J162" s="127"/>
-      <c r="K162" s="127"/>
-      <c r="L162" s="127"/>
-      <c r="M162" s="127"/>
-      <c r="N162" s="127"/>
+      <c r="C162" s="123"/>
+      <c r="D162" s="123"/>
+      <c r="E162" s="123"/>
+      <c r="F162" s="123"/>
+      <c r="G162" s="123"/>
+      <c r="H162" s="123"/>
+      <c r="I162" s="123"/>
+      <c r="J162" s="123"/>
+      <c r="K162" s="123"/>
+      <c r="L162" s="123"/>
+      <c r="M162" s="123"/>
+      <c r="N162" s="123"/>
     </row>
     <row r="163" spans="2:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>

</xml_diff>

<commit_message>
added timer... will implement quiz
</commit_message>
<xml_diff>
--- a/General Test.xlsx
+++ b/General Test.xlsx
@@ -6462,9 +6462,6 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="justify" wrapText="1"/>
     </xf>
@@ -6527,6 +6524,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7333,7 +7333,7 @@
       <c r="E2" s="85"/>
       <c r="F2" s="86">
         <f ca="1">TODAY()</f>
-        <v>42915</v>
+        <v>42916</v>
       </c>
       <c r="G2" s="85"/>
       <c r="H2" s="77"/>
@@ -7521,8 +7521,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B285" sqref="B285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11082,20 +11082,20 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="110" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="110"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
@@ -11857,158 +11857,158 @@
       <c r="E66" s="4"/>
     </row>
     <row r="67" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="123" t="s">
+      <c r="B67" s="122" t="s">
         <v>460</v>
       </c>
-      <c r="C67" s="123"/>
-      <c r="D67" s="123"/>
-      <c r="E67" s="123"/>
-      <c r="F67" s="123"/>
-      <c r="G67" s="123"/>
-      <c r="H67" s="123"/>
-      <c r="I67" s="123"/>
-      <c r="J67" s="123"/>
-      <c r="K67" s="123"/>
+      <c r="C67" s="122"/>
+      <c r="D67" s="122"/>
+      <c r="E67" s="122"/>
+      <c r="F67" s="122"/>
+      <c r="G67" s="122"/>
+      <c r="H67" s="122"/>
+      <c r="I67" s="122"/>
+      <c r="J67" s="122"/>
+      <c r="K67" s="122"/>
     </row>
     <row r="68" spans="1:12" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="111" t="s">
+      <c r="B68" s="110" t="s">
         <v>461</v>
       </c>
-      <c r="C68" s="111"/>
-      <c r="D68" s="111"/>
-      <c r="E68" s="111"/>
-      <c r="F68" s="111"/>
-      <c r="G68" s="111"/>
-      <c r="H68" s="111"/>
-      <c r="I68" s="111"/>
-      <c r="J68" s="111"/>
-      <c r="K68" s="111"/>
+      <c r="C68" s="110"/>
+      <c r="D68" s="110"/>
+      <c r="E68" s="110"/>
+      <c r="F68" s="110"/>
+      <c r="G68" s="110"/>
+      <c r="H68" s="110"/>
+      <c r="I68" s="110"/>
+      <c r="J68" s="110"/>
+      <c r="K68" s="110"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C69" s="112">
+      <c r="C69" s="111">
         <v>1</v>
       </c>
-      <c r="D69" s="132" t="s">
+      <c r="D69" s="131" t="s">
         <v>463</v>
       </c>
-      <c r="E69" s="133"/>
-      <c r="F69" s="133"/>
-      <c r="G69" s="133"/>
-      <c r="H69" s="133"/>
-      <c r="I69" s="133"/>
-      <c r="J69" s="133"/>
-      <c r="K69" s="134"/>
+      <c r="E69" s="132"/>
+      <c r="F69" s="132"/>
+      <c r="G69" s="132"/>
+      <c r="H69" s="132"/>
+      <c r="I69" s="132"/>
+      <c r="J69" s="132"/>
+      <c r="K69" s="133"/>
     </row>
     <row r="70" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C70" s="113"/>
-      <c r="D70" s="117" t="s">
+      <c r="C70" s="112"/>
+      <c r="D70" s="116" t="s">
         <v>464</v>
       </c>
-      <c r="E70" s="118"/>
-      <c r="F70" s="118"/>
-      <c r="G70" s="118"/>
-      <c r="H70" s="118"/>
-      <c r="I70" s="118"/>
-      <c r="J70" s="118"/>
-      <c r="K70" s="119"/>
+      <c r="E70" s="117"/>
+      <c r="F70" s="117"/>
+      <c r="G70" s="117"/>
+      <c r="H70" s="117"/>
+      <c r="I70" s="117"/>
+      <c r="J70" s="117"/>
+      <c r="K70" s="118"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C71" s="112">
+      <c r="C71" s="111">
         <v>2</v>
       </c>
-      <c r="D71" s="120" t="s">
+      <c r="D71" s="119" t="s">
         <v>465</v>
       </c>
-      <c r="E71" s="121"/>
-      <c r="F71" s="121"/>
-      <c r="G71" s="121"/>
-      <c r="H71" s="121"/>
-      <c r="I71" s="121"/>
-      <c r="J71" s="121"/>
-      <c r="K71" s="122"/>
+      <c r="E71" s="120"/>
+      <c r="F71" s="120"/>
+      <c r="G71" s="120"/>
+      <c r="H71" s="120"/>
+      <c r="I71" s="120"/>
+      <c r="J71" s="120"/>
+      <c r="K71" s="121"/>
     </row>
     <row r="72" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="113"/>
-      <c r="D72" s="117" t="s">
+      <c r="C72" s="112"/>
+      <c r="D72" s="116" t="s">
         <v>464</v>
       </c>
-      <c r="E72" s="118"/>
-      <c r="F72" s="118"/>
-      <c r="G72" s="118"/>
-      <c r="H72" s="118"/>
-      <c r="I72" s="118"/>
-      <c r="J72" s="118"/>
-      <c r="K72" s="119"/>
+      <c r="E72" s="117"/>
+      <c r="F72" s="117"/>
+      <c r="G72" s="117"/>
+      <c r="H72" s="117"/>
+      <c r="I72" s="117"/>
+      <c r="J72" s="117"/>
+      <c r="K72" s="118"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="112">
+      <c r="C73" s="111">
         <v>3</v>
       </c>
-      <c r="D73" s="129" t="s">
+      <c r="D73" s="128" t="s">
         <v>466</v>
       </c>
-      <c r="E73" s="130"/>
-      <c r="F73" s="130"/>
-      <c r="G73" s="130"/>
-      <c r="H73" s="130"/>
-      <c r="I73" s="130"/>
-      <c r="J73" s="130"/>
-      <c r="K73" s="131"/>
+      <c r="E73" s="129"/>
+      <c r="F73" s="129"/>
+      <c r="G73" s="129"/>
+      <c r="H73" s="129"/>
+      <c r="I73" s="129"/>
+      <c r="J73" s="129"/>
+      <c r="K73" s="130"/>
     </row>
     <row r="74" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C74" s="113"/>
-      <c r="D74" s="124" t="s">
+      <c r="C74" s="112"/>
+      <c r="D74" s="123" t="s">
         <v>467</v>
       </c>
-      <c r="E74" s="125"/>
-      <c r="F74" s="125"/>
-      <c r="G74" s="125"/>
-      <c r="H74" s="125"/>
-      <c r="I74" s="125"/>
-      <c r="J74" s="125"/>
+      <c r="E74" s="124"/>
+      <c r="F74" s="124"/>
+      <c r="G74" s="124"/>
+      <c r="H74" s="124"/>
+      <c r="I74" s="124"/>
+      <c r="J74" s="124"/>
       <c r="K74" s="15"/>
     </row>
     <row r="75" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="26">
         <v>4</v>
       </c>
-      <c r="D75" s="114" t="s">
+      <c r="D75" s="113" t="s">
         <v>462</v>
       </c>
-      <c r="E75" s="115"/>
-      <c r="F75" s="115"/>
-      <c r="G75" s="115"/>
-      <c r="H75" s="115"/>
-      <c r="I75" s="115"/>
-      <c r="J75" s="115"/>
-      <c r="K75" s="116"/>
+      <c r="E75" s="114"/>
+      <c r="F75" s="114"/>
+      <c r="G75" s="114"/>
+      <c r="H75" s="114"/>
+      <c r="I75" s="114"/>
+      <c r="J75" s="114"/>
+      <c r="K75" s="115"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C76" s="112">
+      <c r="C76" s="111">
         <v>5</v>
       </c>
-      <c r="D76" s="126" t="s">
+      <c r="D76" s="125" t="s">
         <v>468</v>
       </c>
-      <c r="E76" s="127"/>
-      <c r="F76" s="127"/>
-      <c r="G76" s="127"/>
-      <c r="H76" s="127"/>
-      <c r="I76" s="127"/>
-      <c r="J76" s="127"/>
-      <c r="K76" s="128"/>
+      <c r="E76" s="126"/>
+      <c r="F76" s="126"/>
+      <c r="G76" s="126"/>
+      <c r="H76" s="126"/>
+      <c r="I76" s="126"/>
+      <c r="J76" s="126"/>
+      <c r="K76" s="127"/>
     </row>
     <row r="77" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="113"/>
-      <c r="D77" s="124" t="s">
+      <c r="C77" s="112"/>
+      <c r="D77" s="123" t="s">
         <v>469</v>
       </c>
-      <c r="E77" s="125"/>
-      <c r="F77" s="125"/>
-      <c r="G77" s="125"/>
-      <c r="H77" s="125"/>
-      <c r="I77" s="125"/>
-      <c r="J77" s="125"/>
+      <c r="E77" s="124"/>
+      <c r="F77" s="124"/>
+      <c r="G77" s="124"/>
+      <c r="H77" s="124"/>
+      <c r="I77" s="124"/>
+      <c r="J77" s="124"/>
       <c r="K77" s="15"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -12035,30 +12035,30 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D83" s="135" t="s">
+      <c r="D83" s="134" t="s">
         <v>473</v>
       </c>
-      <c r="E83" s="135"/>
-      <c r="F83" s="135"/>
-      <c r="G83" s="135"/>
-      <c r="H83" s="135"/>
-      <c r="I83" s="135"/>
-      <c r="J83" s="135"/>
-      <c r="K83" s="135"/>
-      <c r="L83" s="135"/>
+      <c r="E83" s="134"/>
+      <c r="F83" s="134"/>
+      <c r="G83" s="134"/>
+      <c r="H83" s="134"/>
+      <c r="I83" s="134"/>
+      <c r="J83" s="134"/>
+      <c r="K83" s="134"/>
+      <c r="L83" s="134"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D84" s="110" t="s">
+      <c r="D84" s="135" t="s">
         <v>474</v>
       </c>
-      <c r="E84" s="110"/>
-      <c r="F84" s="110"/>
-      <c r="G84" s="110"/>
-      <c r="H84" s="110"/>
-      <c r="I84" s="110"/>
-      <c r="J84" s="110"/>
-      <c r="K84" s="110"/>
-      <c r="L84" s="110"/>
+      <c r="E84" s="135"/>
+      <c r="F84" s="135"/>
+      <c r="G84" s="135"/>
+      <c r="H84" s="135"/>
+      <c r="I84" s="135"/>
+      <c r="J84" s="135"/>
+      <c r="K84" s="135"/>
+      <c r="L84" s="135"/>
     </row>
     <row r="86" spans="1:12" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="3"/>
@@ -12345,7 +12345,6 @@
   </sheetData>
   <sheetProtection password="D855" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="D69:K69"/>
     <mergeCell ref="D83:L83"/>
     <mergeCell ref="D84:L84"/>
     <mergeCell ref="B3:M3"/>
@@ -12363,6 +12362,7 @@
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="D70:K70"/>
+    <mergeCell ref="D69:K69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" orientation="portrait" r:id="rId1"/>
@@ -14993,21 +14993,21 @@
       </c>
     </row>
     <row r="3" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="122" t="s">
         <v>760</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="123"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
     </row>
     <row r="4" spans="2:14" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="37"/>
@@ -15024,21 +15024,21 @@
       <c r="M4" s="37"/>
     </row>
     <row r="5" spans="2:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="110" t="s">
         <v>761</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="111"/>
-      <c r="N5" s="111"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="110"/>
+      <c r="M5" s="110"/>
+      <c r="N5" s="110"/>
     </row>
     <row r="6" spans="2:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
@@ -15199,21 +15199,21 @@
       </c>
     </row>
     <row r="76" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="123" t="s">
+      <c r="B76" s="122" t="s">
         <v>764</v>
       </c>
-      <c r="C76" s="123"/>
-      <c r="D76" s="123"/>
-      <c r="E76" s="123"/>
-      <c r="F76" s="123"/>
-      <c r="G76" s="123"/>
-      <c r="H76" s="123"/>
-      <c r="I76" s="123"/>
-      <c r="J76" s="123"/>
-      <c r="K76" s="123"/>
-      <c r="L76" s="123"/>
-      <c r="M76" s="123"/>
-      <c r="N76" s="123"/>
+      <c r="C76" s="122"/>
+      <c r="D76" s="122"/>
+      <c r="E76" s="122"/>
+      <c r="F76" s="122"/>
+      <c r="G76" s="122"/>
+      <c r="H76" s="122"/>
+      <c r="I76" s="122"/>
+      <c r="J76" s="122"/>
+      <c r="K76" s="122"/>
+      <c r="L76" s="122"/>
+      <c r="M76" s="122"/>
+      <c r="N76" s="122"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B77" s="37"/>
@@ -15230,21 +15230,21 @@
       <c r="M77" s="37"/>
     </row>
     <row r="78" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="111" t="s">
+      <c r="B78" s="110" t="s">
         <v>765</v>
       </c>
-      <c r="C78" s="111"/>
-      <c r="D78" s="111"/>
-      <c r="E78" s="111"/>
-      <c r="F78" s="111"/>
-      <c r="G78" s="111"/>
-      <c r="H78" s="111"/>
-      <c r="I78" s="111"/>
-      <c r="J78" s="111"/>
-      <c r="K78" s="111"/>
-      <c r="L78" s="111"/>
-      <c r="M78" s="111"/>
-      <c r="N78" s="111"/>
+      <c r="C78" s="110"/>
+      <c r="D78" s="110"/>
+      <c r="E78" s="110"/>
+      <c r="F78" s="110"/>
+      <c r="G78" s="110"/>
+      <c r="H78" s="110"/>
+      <c r="I78" s="110"/>
+      <c r="J78" s="110"/>
+      <c r="K78" s="110"/>
+      <c r="L78" s="110"/>
+      <c r="M78" s="110"/>
+      <c r="N78" s="110"/>
     </row>
     <row r="79" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="9" t="s">
@@ -15299,21 +15299,21 @@
       </c>
     </row>
     <row r="117" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="111" t="s">
+      <c r="B117" s="110" t="s">
         <v>767</v>
       </c>
-      <c r="C117" s="111"/>
-      <c r="D117" s="111"/>
-      <c r="E117" s="111"/>
-      <c r="F117" s="111"/>
-      <c r="G117" s="111"/>
-      <c r="H117" s="111"/>
-      <c r="I117" s="111"/>
-      <c r="J117" s="111"/>
-      <c r="K117" s="111"/>
-      <c r="L117" s="111"/>
-      <c r="M117" s="111"/>
-      <c r="N117" s="111"/>
+      <c r="C117" s="110"/>
+      <c r="D117" s="110"/>
+      <c r="E117" s="110"/>
+      <c r="F117" s="110"/>
+      <c r="G117" s="110"/>
+      <c r="H117" s="110"/>
+      <c r="I117" s="110"/>
+      <c r="J117" s="110"/>
+      <c r="K117" s="110"/>
+      <c r="L117" s="110"/>
+      <c r="M117" s="110"/>
+      <c r="N117" s="110"/>
     </row>
     <row r="118" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="9" t="s">
@@ -15380,21 +15380,21 @@
       </c>
     </row>
     <row r="162" spans="2:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="123" t="s">
+      <c r="B162" s="122" t="s">
         <v>769</v>
       </c>
-      <c r="C162" s="123"/>
-      <c r="D162" s="123"/>
-      <c r="E162" s="123"/>
-      <c r="F162" s="123"/>
-      <c r="G162" s="123"/>
-      <c r="H162" s="123"/>
-      <c r="I162" s="123"/>
-      <c r="J162" s="123"/>
-      <c r="K162" s="123"/>
-      <c r="L162" s="123"/>
-      <c r="M162" s="123"/>
-      <c r="N162" s="123"/>
+      <c r="C162" s="122"/>
+      <c r="D162" s="122"/>
+      <c r="E162" s="122"/>
+      <c r="F162" s="122"/>
+      <c r="G162" s="122"/>
+      <c r="H162" s="122"/>
+      <c r="I162" s="122"/>
+      <c r="J162" s="122"/>
+      <c r="K162" s="122"/>
+      <c r="L162" s="122"/>
+      <c r="M162" s="122"/>
+      <c r="N162" s="122"/>
     </row>
     <row r="163" spans="2:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>

</xml_diff>